<commit_message>
Forecastings done and results worksheet
</commit_message>
<xml_diff>
--- a/Excel divisiones/GICIS308.xlsx
+++ b/Excel divisiones/GICIS308.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/if710183_iteso_mx/Documents/IFI/8 Octavo/PAP/Plantas_Intermitentes/Excel divisiones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_DB96A9210F8410A2B218CF5AA06B796F60BEEE8E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FFF39FA-0E77-D444-8A6D-0A46A69E8EC9}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_DB96A9210F8410A2B218CF5AA06B796F60BEEE8E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C32FA5DE-2563-5D4A-AD9A-D71B41DDAB1A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -495,11 +495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2309"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2276" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I2306" sqref="I2306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>